<commit_message>
Finale Map ausgewählt und Regeln weiter bearbeitet
</commit_message>
<xml_diff>
--- a/Charaktere/Chrakterbogen.xlsx
+++ b/Charaktere/Chrakterbogen.xlsx
@@ -22,7 +22,9 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Grunddaten!$A$1:$K$49</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Waffentalente!$A$1:$M$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Grunddaten!$A$1:$K$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Grunddaten!$A$1:$K$49</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Waffentalente!$A$1:$M$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">Waffentalente!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -36,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="203">
   <si>
-    <t xml:space="preserve">Orcerta</t>
+    <t xml:space="preserve">Duerratan</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -1200,13 +1202,13 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2644,10 +2646,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="9.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="16" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="16" style="0" width="9.13"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="21" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="39" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Map Sugewählt und Regeln weiter ausgefeilt
</commit_message>
<xml_diff>
--- a/Charaktere/Chrakterbogen.xlsx
+++ b/Charaktere/Chrakterbogen.xlsx
@@ -22,7 +22,9 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Grunddaten!$A$1:$K$49</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Waffentalente!$A$1:$M$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Grunddaten!$A$1:$K$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Grunddaten!$A$1:$K$49</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">Waffentalente!$A$1:$M$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area_0" vbProcedure="false">Waffentalente!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -36,7 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="203">
   <si>
-    <t xml:space="preserve">Orcerta</t>
+    <t xml:space="preserve">Duerratan</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -1200,13 +1202,13 @@
   <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2644,10 +2646,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="9.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="16" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="1" style="0" width="9.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="16" style="0" width="9.13"/>
     <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="21" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" s="39" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>